<commit_message>
added systems of gov
</commit_message>
<xml_diff>
--- a/Data/raw_data_master_list.xlsx
+++ b/Data/raw_data_master_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chitwan/Documents/GTA docs/6242/6242Project/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C95F649-2DD4-994D-95D4-8BF5484F836D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B8BB5D1-CC40-624E-B99D-4564F37FD158}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14420" xr2:uid="{31E375E8-A733-1144-AAE7-CD79965017D1}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Dataset Name</t>
   </si>
@@ -70,13 +70,25 @@
   </si>
   <si>
     <t>1960-2017</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/List_of_countries_by_system_of_government</t>
+  </si>
+  <si>
+    <t>system_of_gov</t>
+  </si>
+  <si>
+    <t>wikipedia article of systems of government (democracy, chiefdom, etc.) for all UN countries</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -88,6 +100,14 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -119,14 +139,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -439,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB703161-5D44-6C49-8AB5-0143908753DB}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -452,7 +476,7 @@
     <col min="5" max="5" width="47.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -468,8 +492,11 @@
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="F1" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -486,7 +513,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -500,7 +527,21 @@
         <v>7</v>
       </c>
     </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F4" r:id="rId1" xr:uid="{75BB88A6-7CE1-924F-B417-8D80E10C8215}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adding years of schooling
</commit_message>
<xml_diff>
--- a/Data/raw_data_master_list.xlsx
+++ b/Data/raw_data_master_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chitwan/Documents/GTA docs/6242/6242Project/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B8BB5D1-CC40-624E-B99D-4564F37FD158}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D200DD6-A3AE-464A-87F6-5AA2B07CB061}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14420" xr2:uid="{31E375E8-A733-1144-AAE7-CD79965017D1}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>Dataset Name</t>
   </si>
@@ -82,6 +82,15 @@
   </si>
   <si>
     <t>wikipedia article of systems of government (democracy, chiefdom, etc.) for all UN countries</t>
+  </si>
+  <si>
+    <t>mean_years_of_schooling</t>
+  </si>
+  <si>
+    <t>average years of sccooling per country</t>
+  </si>
+  <si>
+    <t>1870-2017</t>
   </si>
 </sst>
 </file>
@@ -463,10 +472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB703161-5D44-6C49-8AB5-0143908753DB}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -538,6 +547,20 @@
         <v>14</v>
       </c>
     </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F4" r:id="rId1" xr:uid="{75BB88A6-7CE1-924F-B417-8D80E10C8215}"/>

</xml_diff>